<commit_message>
updated BLE_notify sketch and Services spreadsheet
</commit_message>
<xml_diff>
--- a/arduino/Bluetooth/Dashboard BLE Services.xlsx
+++ b/arduino/Bluetooth/Dashboard BLE Services.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sutdapac-my.sharepoint.com/personal/nigel_gomes_mymail_sutd_edu_sg/Documents/Documents/GitHub/evam-dashboard/arduino/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sutdapac-my.sharepoint.com/personal/nigel_gomes_mymail_sutd_edu_sg/Documents/Documents/GitHub/evam-dashboard/arduino/Bluetooth/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="132" documentId="8_{4D1D99D6-6873-4CBD-8EFB-7BCD47A27D5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F08A46D8-A20B-406D-AB26-63F98EB19ADA}"/>
+  <xr:revisionPtr revIDLastSave="178" documentId="8_{4D1D99D6-6873-4CBD-8EFB-7BCD47A27D5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5523F9D0-12BA-4229-9F68-4E307014940B}"/>
   <bookViews>
     <workbookView xWindow="1534" yWindow="-103" windowWidth="42455" windowHeight="24892" xr2:uid="{07500EA1-3706-482B-9C71-1920CA5A2111}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="65">
   <si>
     <t>Service</t>
   </si>
@@ -129,24 +129,6 @@
     <t>Read | Notify</t>
   </si>
   <si>
-    <t>Throttle %</t>
-  </si>
-  <si>
-    <t>Brake %</t>
-  </si>
-  <si>
-    <t>Batt %</t>
-  </si>
-  <si>
-    <t>Batt Voltage (V)</t>
-  </si>
-  <si>
-    <t>Batt Current (A)</t>
-  </si>
-  <si>
-    <t>Batt Temp (deg C)</t>
-  </si>
-  <si>
     <t>Car Status</t>
   </si>
   <si>
@@ -189,24 +171,9 @@
     <t>Lighting</t>
   </si>
   <si>
-    <t>Front Lights</t>
-  </si>
-  <si>
     <t>Read | Write</t>
   </si>
   <si>
-    <t>Hex Colour Value (eg #101010, but without the hashtag)</t>
-  </si>
-  <si>
-    <t>Rear Lights</t>
-  </si>
-  <si>
-    <t>Hex Colour Value</t>
-  </si>
-  <si>
-    <t>Interior Lights</t>
-  </si>
-  <si>
     <t>Indicator</t>
   </si>
   <si>
@@ -222,23 +189,53 @@
     <t>Forward = 0 Reverse = 1</t>
   </si>
   <si>
-    <t>2 bytes can be combined for data range of 0-65535. For now we're not combining</t>
-  </si>
-  <si>
-    <t>Speed (in km/h) 0-255</t>
-  </si>
-  <si>
     <t>Other Screens</t>
   </si>
   <si>
     <t>Angle (in deg) = raw data-128</t>
+  </si>
+  <si>
+    <t>Speed (in km/h) = raw data (0-255)</t>
+  </si>
+  <si>
+    <t>Throttle % = raw data (0-100)</t>
+  </si>
+  <si>
+    <t>Brake % = raw data (0-100)</t>
+  </si>
+  <si>
+    <t>Batt % = raw data (0-100)</t>
+  </si>
+  <si>
+    <t>Batt Temp (deg C) = raw data (0-255)</t>
+  </si>
+  <si>
+    <t>Batt Voltage (V) = raw data (0-255)</t>
+  </si>
+  <si>
+    <t>2 bytes can be combined for data range of 0-65535</t>
+  </si>
+  <si>
+    <t>Batt Current (A) = (MSB * 255 + LSB)/100 (range: 0-65535)</t>
+  </si>
+  <si>
+    <t>Front: Hex Colour Value (eg #101010, but without the hashtag)</t>
+  </si>
+  <si>
+    <t>Rear: Hex Colour Value (eg #101010, but without the hashtag)</t>
+  </si>
+  <si>
+    <t>Interior: Hex Colour Value (eg #101010, but without the hashtag)</t>
+  </si>
+  <si>
+    <t>Lights</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -264,6 +261,28 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.34998626667073579"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -295,7 +314,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -332,12 +351,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
@@ -361,7 +389,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -370,14 +408,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
@@ -696,7 +737,7 @@
   <dimension ref="A1:Y23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -706,7 +747,15 @@
     <col min="3" max="3" width="0.69140625" style="8" customWidth="1"/>
     <col min="4" max="4" width="20.53515625" customWidth="1"/>
     <col min="5" max="5" width="1" style="8" customWidth="1"/>
-    <col min="6" max="25" width="16.3046875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="30.3828125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="26.53515625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="23" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.07421875" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="29.53515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="35.4609375" style="4" customWidth="1"/>
+    <col min="12" max="12" width="22.15234375" style="4" customWidth="1"/>
+    <col min="13" max="13" width="31.3828125" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="25" width="16.3046875" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" s="1" customFormat="1" ht="16.75" x14ac:dyDescent="0.45">
@@ -716,28 +765,28 @@
       <c r="B1" s="3"/>
       <c r="C1" s="6"/>
       <c r="E1" s="6"/>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="17"/>
-      <c r="S1" s="17"/>
-      <c r="T1" s="17"/>
-      <c r="U1" s="17"/>
-      <c r="V1" s="17"/>
-      <c r="W1" s="17"/>
-      <c r="X1" s="17"/>
-      <c r="Y1" s="17"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
+      <c r="Q1" s="23"/>
+      <c r="R1" s="23"/>
+      <c r="S1" s="23"/>
+      <c r="T1" s="23"/>
+      <c r="U1" s="23"/>
+      <c r="V1" s="23"/>
+      <c r="W1" s="23"/>
+      <c r="X1" s="23"/>
+      <c r="Y1" s="23"/>
     </row>
     <row r="2" spans="1:25" s="2" customFormat="1" ht="17.149999999999999" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B2" s="2" t="s">
@@ -810,10 +859,10 @@
       </c>
     </row>
     <row r="3" spans="1:25" s="12" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="21"/>
+      <c r="B3" s="17"/>
       <c r="C3" s="13"/>
       <c r="E3" s="13"/>
       <c r="F3" s="14"/>
@@ -838,39 +887,39 @@
       <c r="Y3" s="14"/>
     </row>
     <row r="4" spans="1:25" ht="44.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="18"/>
-      <c r="B4" s="18" t="s">
+      <c r="A4" s="15"/>
+      <c r="B4" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="19" t="s">
+      <c r="F4" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="G4" s="19" t="s">
+      <c r="G4" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="H4" s="16"/>
+      <c r="I4" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="H4" s="19"/>
-      <c r="I4" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="J4" s="20"/>
-      <c r="K4" s="19"/>
-      <c r="L4" s="19"/>
-      <c r="M4" s="19"/>
-      <c r="N4" s="19"/>
-      <c r="O4" s="19"/>
-      <c r="P4" s="19"/>
-      <c r="Q4" s="19"/>
-      <c r="R4" s="19"/>
-      <c r="S4" s="19"/>
-      <c r="T4" s="19"/>
-      <c r="U4" s="19"/>
-      <c r="V4" s="19"/>
-      <c r="W4" s="19"/>
-      <c r="X4" s="19"/>
-      <c r="Y4" s="19"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="16"/>
+      <c r="P4" s="16"/>
+      <c r="Q4" s="16"/>
+      <c r="R4" s="16"/>
+      <c r="S4" s="16"/>
+      <c r="T4" s="16"/>
+      <c r="U4" s="16"/>
+      <c r="V4" s="16"/>
+      <c r="W4" s="16"/>
+      <c r="X4" s="16"/>
+      <c r="Y4" s="16"/>
     </row>
     <row r="7" spans="1:25" s="9" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A7" s="9" t="s">
@@ -907,50 +956,53 @@
         <v>30</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="G8" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="K8" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="L8" s="25"/>
+      <c r="M8" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="B9" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="C9" s="27"/>
+      <c r="D9" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="27"/>
+      <c r="F9" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="G9" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="H9" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="I9" s="28" t="s">
         <v>33</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="K8" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="L8" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:25" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="B9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D9" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:25" s="9" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A11" s="9" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="C11" s="10"/>
       <c r="E11" s="10"/>
@@ -976,61 +1028,78 @@
       <c r="Y11" s="11"/>
     </row>
     <row r="12" spans="1:25" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B12" t="s">
+      <c r="B12" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="19"/>
+      <c r="D12" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="19"/>
+      <c r="F12" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="B13" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="19"/>
+      <c r="D13" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="19"/>
+      <c r="F13" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="G13" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="H13" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="I13" s="20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="B14" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="D12" t="s">
+      <c r="C14" s="19"/>
+      <c r="D14" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="F12" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="B13" t="s">
+      <c r="E14" s="19"/>
+      <c r="F14" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="D13" t="s">
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="B15" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="19"/>
+      <c r="D15" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="F13" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="G13" s="4" t="s">
+      <c r="E15" s="19"/>
+      <c r="F15" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="H13" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="I13" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="14" spans="1:25" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="B14" t="s">
-        <v>46</v>
-      </c>
-      <c r="D14" t="s">
-        <v>30</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="B15" t="s">
-        <v>48</v>
-      </c>
-      <c r="D15" t="s">
-        <v>30</v>
-      </c>
-      <c r="F15" s="15" t="s">
-        <v>49</v>
-      </c>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
     </row>
     <row r="19" spans="1:25" s="9" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A19" s="9" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C19" s="10"/>
       <c r="E19" s="10"/>
@@ -1057,61 +1126,60 @@
     </row>
     <row r="20" spans="1:25" ht="32.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B20" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="D20" t="s">
-        <v>52</v>
-      </c>
-      <c r="F20" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="G20" s="16"/>
-      <c r="H20" s="16"/>
+        <v>45</v>
+      </c>
+      <c r="F20" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="G20" s="22"/>
+      <c r="H20" s="22"/>
+      <c r="I20" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="J20" s="22"/>
+      <c r="K20" s="22"/>
+      <c r="L20" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="M20" s="22"/>
+      <c r="N20" s="22"/>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="B21" t="s">
-        <v>54</v>
-      </c>
-      <c r="D21" t="s">
-        <v>52</v>
-      </c>
-      <c r="F21" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="G21" s="16"/>
-      <c r="H21" s="16"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="22"/>
+      <c r="H21" s="22"/>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="B22" t="s">
-        <v>56</v>
-      </c>
-      <c r="D22" t="s">
-        <v>52</v>
-      </c>
-      <c r="F22" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
-    </row>
-    <row r="23" spans="1:25" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="B23" t="s">
-        <v>57</v>
-      </c>
-      <c r="D23" t="s">
-        <v>52</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>58</v>
+      <c r="F22" s="22"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="22"/>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="B23" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" s="27"/>
+      <c r="D23" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="E23" s="27"/>
+      <c r="F23" s="28" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="8">
     <mergeCell ref="F22:H22"/>
     <mergeCell ref="F1:Y1"/>
     <mergeCell ref="I4:J4"/>
     <mergeCell ref="F20:H20"/>
     <mergeCell ref="F21:H21"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="I20:K20"/>
+    <mergeCell ref="L20:N20"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Improved battery statistics and screen layout
</commit_message>
<xml_diff>
--- a/arduino/Bluetooth/Dashboard BLE Services.xlsx
+++ b/arduino/Bluetooth/Dashboard BLE Services.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sutdapac-my.sharepoint.com/personal/nigel_gomes_mymail_sutd_edu_sg/Documents/Documents/GitHub/evam-dashboard/arduino/Bluetooth/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\evam-dashboard\arduino\Bluetooth\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="178" documentId="8_{4D1D99D6-6873-4CBD-8EFB-7BCD47A27D5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5523F9D0-12BA-4229-9F68-4E307014940B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{615FDA87-1878-4193-8D05-02AAAAB35188}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1534" yWindow="-103" windowWidth="42455" windowHeight="24892" xr2:uid="{07500EA1-3706-482B-9C71-1920CA5A2111}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{07500EA1-3706-482B-9C71-1920CA5A2111}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="69">
   <si>
     <t>Service</t>
   </si>
@@ -189,9 +189,6 @@
     <t>Forward = 0 Reverse = 1</t>
   </si>
   <si>
-    <t>Other Screens</t>
-  </si>
-  <si>
     <t>Angle (in deg) = raw data-128</t>
   </si>
   <si>
@@ -229,6 +226,21 @@
   </si>
   <si>
     <t>Lights</t>
+  </si>
+  <si>
+    <t>4fafc201-1fb5-459e-8fcc-c5c9c331914b</t>
+  </si>
+  <si>
+    <t>beb5483e-36e1-4688-b7f5-ea07361b26a8</t>
+  </si>
+  <si>
+    <t>5d2e6e74-31f0-445e-8088-827c53b71166</t>
+  </si>
+  <si>
+    <t>825eef3b-e3d0-4ca6-bef7-6428b7260f35</t>
+  </si>
+  <si>
+    <t>Status</t>
   </si>
 </sst>
 </file>
@@ -288,18 +300,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="1" tint="0.34998626667073579"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -365,7 +371,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
@@ -376,30 +382,28 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -408,16 +412,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -734,455 +733,440 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8933487E-7BF6-40CC-8C7B-EEF7163D084A}">
-  <dimension ref="A1:Y23"/>
+  <dimension ref="A1:W23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.53515625" customWidth="1"/>
-    <col min="2" max="2" width="28.3828125" customWidth="1"/>
-    <col min="3" max="3" width="0.69140625" style="8" customWidth="1"/>
-    <col min="4" max="4" width="20.53515625" customWidth="1"/>
-    <col min="5" max="5" width="1" style="8" customWidth="1"/>
-    <col min="6" max="6" width="30.3828125" style="4" customWidth="1"/>
-    <col min="7" max="7" width="26.53515625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="23" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="31.07421875" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="29.53515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="35.4609375" style="4" customWidth="1"/>
-    <col min="12" max="12" width="22.15234375" style="4" customWidth="1"/>
-    <col min="13" max="13" width="31.3828125" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="25" width="16.3046875" style="4" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" customWidth="1"/>
+    <col min="2" max="2" width="42" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" customWidth="1"/>
+    <col min="4" max="4" width="30.42578125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="26.5703125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="23" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="35.42578125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="22.140625" style="4" customWidth="1"/>
+    <col min="11" max="11" width="31.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="23" width="16.28515625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="1" customFormat="1" ht="16.75" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:23" s="1" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="23" t="s">
+      <c r="B1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23"/>
-      <c r="N1" s="23"/>
-      <c r="O1" s="23"/>
-      <c r="P1" s="23"/>
-      <c r="Q1" s="23"/>
-      <c r="R1" s="23"/>
-      <c r="S1" s="23"/>
-      <c r="T1" s="23"/>
-      <c r="U1" s="23"/>
-      <c r="V1" s="23"/>
-      <c r="W1" s="23"/>
-      <c r="X1" s="23"/>
-      <c r="Y1" s="23"/>
-    </row>
-    <row r="2" spans="1:25" s="2" customFormat="1" ht="17.149999999999999" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
+      <c r="P1" s="19"/>
+      <c r="Q1" s="19"/>
+      <c r="R1" s="19"/>
+      <c r="S1" s="19"/>
+      <c r="T1" s="19"/>
+      <c r="U1" s="19"/>
+      <c r="V1" s="19"/>
+      <c r="W1" s="19"/>
+    </row>
+    <row r="2" spans="1:23" s="2" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="7"/>
+      <c r="D2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="F2" s="5" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="R2" s="5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="S2" s="5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="T2" s="5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="U2" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="V2" s="5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="W2" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="X2" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y2" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:25" s="12" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="17" t="s">
+    <row r="3" spans="1:23" s="8" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
-      <c r="O3" s="14"/>
-      <c r="P3" s="14"/>
-      <c r="Q3" s="14"/>
-      <c r="R3" s="14"/>
-      <c r="S3" s="14"/>
-      <c r="T3" s="14"/>
-      <c r="U3" s="14"/>
-      <c r="V3" s="14"/>
-      <c r="W3" s="14"/>
-      <c r="X3" s="14"/>
-      <c r="Y3" s="14"/>
-    </row>
-    <row r="4" spans="1:25" ht="44.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="15"/>
-      <c r="B4" s="15" t="s">
+      <c r="B3" s="12"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="9"/>
+      <c r="R3" s="9"/>
+      <c r="S3" s="9"/>
+      <c r="T3" s="9"/>
+      <c r="U3" s="9"/>
+      <c r="V3" s="9"/>
+      <c r="W3" s="9"/>
+    </row>
+    <row r="4" spans="1:23" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="10"/>
+      <c r="B4" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="C4" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="D4" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="G4" s="16" t="s">
+      <c r="E4" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="H4" s="16"/>
-      <c r="I4" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="J4" s="24"/>
-      <c r="K4" s="16"/>
-      <c r="L4" s="16"/>
-      <c r="M4" s="16"/>
-      <c r="N4" s="16"/>
-      <c r="O4" s="16"/>
-      <c r="P4" s="16"/>
-      <c r="Q4" s="16"/>
-      <c r="R4" s="16"/>
-      <c r="S4" s="16"/>
-      <c r="T4" s="16"/>
-      <c r="U4" s="16"/>
-      <c r="V4" s="16"/>
-      <c r="W4" s="16"/>
-      <c r="X4" s="16"/>
-      <c r="Y4" s="16"/>
-    </row>
-    <row r="7" spans="1:25" s="9" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="9" t="s">
+      <c r="F4" s="11"/>
+      <c r="G4" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="H4" s="20"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="11"/>
+      <c r="Q4" s="11"/>
+      <c r="R4" s="11"/>
+      <c r="S4" s="11"/>
+      <c r="T4" s="11"/>
+      <c r="U4" s="11"/>
+      <c r="V4" s="11"/>
+      <c r="W4" s="11"/>
+    </row>
+    <row r="7" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="11"/>
-      <c r="L7" s="11"/>
-      <c r="M7" s="11"/>
-      <c r="N7" s="11"/>
-      <c r="O7" s="11"/>
-      <c r="P7" s="11"/>
-      <c r="Q7" s="11"/>
-      <c r="R7" s="11"/>
-      <c r="S7" s="11"/>
-      <c r="T7" s="11"/>
-      <c r="U7" s="11"/>
-      <c r="V7" s="11"/>
-      <c r="W7" s="11"/>
-      <c r="X7" s="11"/>
-      <c r="Y7" s="11"/>
-    </row>
-    <row r="8" spans="1:25" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B7" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="7"/>
+      <c r="S7" s="7"/>
+      <c r="T7" s="7"/>
+      <c r="U7" s="7"/>
+      <c r="V7" s="7"/>
+      <c r="W7" s="7"/>
+    </row>
+    <row r="8" spans="1:23" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>29</v>
       </c>
-      <c r="D8" t="s">
+      <c r="C8" t="s">
         <v>30</v>
       </c>
+      <c r="D8" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>53</v>
+      </c>
       <c r="F8" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="I8" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="I8" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="J8" s="21"/>
+      <c r="K8" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="J8" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="K8" s="25" t="s">
+    </row>
+    <row r="9" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+      <c r="B9" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="G9" s="17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="7"/>
+      <c r="R11" s="7"/>
+      <c r="S11" s="7"/>
+      <c r="T11" s="7"/>
+      <c r="U11" s="7"/>
+      <c r="V11" s="7"/>
+      <c r="W11" s="7"/>
+    </row>
+    <row r="12" spans="1:23" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B13" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="G13" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B14" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B15" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+    </row>
+    <row r="19" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="7"/>
+      <c r="O19" s="7"/>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="7"/>
+      <c r="R19" s="7"/>
+      <c r="S19" s="7"/>
+      <c r="T19" s="7"/>
+      <c r="U19" s="7"/>
+      <c r="V19" s="7"/>
+      <c r="W19" s="7"/>
+    </row>
+    <row r="20" spans="1:23" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="L8" s="25"/>
-      <c r="M8" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="9" spans="1:25" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="B9" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="27"/>
-      <c r="D9" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="E9" s="27"/>
-      <c r="F9" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="G9" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="H9" s="28" t="s">
-        <v>50</v>
-      </c>
-      <c r="I9" s="28" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:25" s="9" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="C11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="11"/>
-      <c r="L11" s="11"/>
-      <c r="M11" s="11"/>
-      <c r="N11" s="11"/>
-      <c r="O11" s="11"/>
-      <c r="P11" s="11"/>
-      <c r="Q11" s="11"/>
-      <c r="R11" s="11"/>
-      <c r="S11" s="11"/>
-      <c r="T11" s="11"/>
-      <c r="U11" s="11"/>
-      <c r="V11" s="11"/>
-      <c r="W11" s="11"/>
-      <c r="X11" s="11"/>
-      <c r="Y11" s="11"/>
-    </row>
-    <row r="12" spans="1:25" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" s="19"/>
-      <c r="D12" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="E12" s="19"/>
-      <c r="F12" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="20"/>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="B13" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" s="19"/>
-      <c r="D13" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="E13" s="19"/>
-      <c r="F13" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="G13" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="H13" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="I13" s="20" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:25" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="B14" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14" s="19"/>
-      <c r="D14" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="E14" s="19"/>
-      <c r="F14" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="20"/>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="B15" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="C15" s="19"/>
-      <c r="D15" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="E15" s="19"/>
-      <c r="F15" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
-      <c r="I15" s="20"/>
-    </row>
-    <row r="19" spans="1:25" s="9" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="C19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="11"/>
-      <c r="K19" s="11"/>
-      <c r="L19" s="11"/>
-      <c r="M19" s="11"/>
-      <c r="N19" s="11"/>
-      <c r="O19" s="11"/>
-      <c r="P19" s="11"/>
-      <c r="Q19" s="11"/>
-      <c r="R19" s="11"/>
-      <c r="S19" s="11"/>
-      <c r="T19" s="11"/>
-      <c r="U19" s="11"/>
-      <c r="V19" s="11"/>
-      <c r="W19" s="11"/>
-      <c r="X19" s="11"/>
-      <c r="Y19" s="11"/>
-    </row>
-    <row r="20" spans="1:25" ht="32.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B20" t="s">
-        <v>64</v>
-      </c>
-      <c r="D20" t="s">
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="H20" s="18"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="K20" s="18"/>
+      <c r="L20" s="18"/>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B23" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="F20" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="G20" s="22"/>
-      <c r="H20" s="22"/>
-      <c r="I20" s="22" t="s">
-        <v>62</v>
-      </c>
-      <c r="J20" s="22"/>
-      <c r="K20" s="22"/>
-      <c r="L20" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="M20" s="22"/>
-      <c r="N20" s="22"/>
-    </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="F21" s="22"/>
-      <c r="G21" s="22"/>
-      <c r="H21" s="22"/>
-    </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="F22" s="22"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="22"/>
-    </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="B23" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="C23" s="27"/>
-      <c r="D23" s="26" t="s">
-        <v>45</v>
-      </c>
-      <c r="E23" s="27"/>
-      <c r="F23" s="28" t="s">
+      <c r="D23" s="17" t="s">
         <v>47</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="F1:Y1"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="F21:H21"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="I20:K20"/>
-    <mergeCell ref="L20:N20"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="D1:W1"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="J20:L20"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changes to arduino BLEcode
main.cpp:
-Added variables for lighting and status
-separate functions for updating data and characteristics
-Updated permissions for lighting and status

Dashboard BLE Services:
-updated UUID locations
</commit_message>
<xml_diff>
--- a/arduino/Bluetooth/Dashboard BLE Services.xlsx
+++ b/arduino/Bluetooth/Dashboard BLE Services.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\evam-dashboard\arduino\Bluetooth\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sutdapac-my.sharepoint.com/personal/nigel_gomes_mymail_sutd_edu_sg/Documents/Documents/GitHub/evam-dashboard/arduino/Bluetooth/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{615FDA87-1878-4193-8D05-02AAAAB35188}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{615FDA87-1878-4193-8D05-02AAAAB35188}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5666CF65-FDB3-4253-86D4-0686F553FB2B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{07500EA1-3706-482B-9C71-1920CA5A2111}"/>
+    <workbookView xWindow="26940" yWindow="4320" windowWidth="22875" windowHeight="16470" xr2:uid="{07500EA1-3706-482B-9C71-1920CA5A2111}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="71">
   <si>
     <t>Service</t>
   </si>
@@ -241,6 +241,12 @@
   </si>
   <si>
     <t>Status</t>
+  </si>
+  <si>
+    <t>UUID</t>
+  </si>
+  <si>
+    <t>Node Status</t>
   </si>
 </sst>
 </file>
@@ -733,10 +739,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8933487E-7BF6-40CC-8C7B-EEF7163D084A}">
-  <dimension ref="A1:W23"/>
+  <dimension ref="A1:X24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -753,14 +759,12 @@
     <col min="10" max="10" width="22.140625" style="4" customWidth="1"/>
     <col min="11" max="11" width="31.42578125" style="4" bestFit="1" customWidth="1"/>
     <col min="12" max="23" width="16.28515625" style="4" customWidth="1"/>
+    <col min="24" max="24" width="48.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="1" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" s="1" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>64</v>
       </c>
       <c r="D1" s="19" t="s">
         <v>1</v>
@@ -785,7 +789,7 @@
       <c r="V1" s="19"/>
       <c r="W1" s="19"/>
     </row>
-    <row r="2" spans="1:23" s="2" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:24" s="2" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
@@ -852,8 +856,11 @@
       <c r="W2" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="1:23" s="8" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="X2" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" s="8" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>24</v>
       </c>
@@ -879,7 +886,7 @@
       <c r="V3" s="9"/>
       <c r="W3" s="9"/>
     </row>
-    <row r="4" spans="1:23" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10"/>
       <c r="B4" s="10" t="s">
         <v>25</v>
@@ -914,12 +921,9 @@
       <c r="V4" s="11"/>
       <c r="W4" s="11"/>
     </row>
-    <row r="7" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>28</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>65</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
@@ -941,8 +945,11 @@
       <c r="U7" s="7"/>
       <c r="V7" s="7"/>
       <c r="W7" s="7"/>
-    </row>
-    <row r="8" spans="1:23" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X7" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>29</v>
       </c>
@@ -971,8 +978,11 @@
       <c r="K8" s="4" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="9" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+      <c r="X8" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" s="16" t="s">
         <v>31</v>
       </c>
@@ -992,151 +1002,158 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B10" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+    </row>
+    <row r="12" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B12" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
-      <c r="N11" s="7"/>
-      <c r="O11" s="7"/>
-      <c r="P11" s="7"/>
-      <c r="Q11" s="7"/>
-      <c r="R11" s="7"/>
-      <c r="S11" s="7"/>
-      <c r="T11" s="7"/>
-      <c r="U11" s="7"/>
-      <c r="V11" s="7"/>
-      <c r="W11" s="7"/>
-    </row>
-    <row r="12" spans="1:23" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="13" t="s">
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="7"/>
+      <c r="R12" s="7"/>
+      <c r="S12" s="7"/>
+      <c r="T12" s="7"/>
+      <c r="U12" s="7"/>
+      <c r="V12" s="7"/>
+      <c r="W12" s="7"/>
+    </row>
+    <row r="13" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="13" t="s">
         <v>34</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B13" s="13" t="s">
-        <v>35</v>
       </c>
       <c r="C13" s="13" t="s">
         <v>30</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="E13" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="F13" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="G13" s="14" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B14" s="13" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C14" s="13" t="s">
         <v>30</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="G14" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B15" s="13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C15" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="15" t="s">
-        <v>43</v>
+      <c r="D15" s="14" t="s">
+        <v>41</v>
       </c>
       <c r="E15" s="14"/>
       <c r="F15" s="14"/>
       <c r="G15" s="14"/>
     </row>
-    <row r="19" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B16" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+    </row>
+    <row r="20" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B20" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="7"/>
-      <c r="L19" s="7"/>
-      <c r="M19" s="7"/>
-      <c r="N19" s="7"/>
-      <c r="O19" s="7"/>
-      <c r="P19" s="7"/>
-      <c r="Q19" s="7"/>
-      <c r="R19" s="7"/>
-      <c r="S19" s="7"/>
-      <c r="T19" s="7"/>
-      <c r="U19" s="7"/>
-      <c r="V19" s="7"/>
-      <c r="W19" s="7"/>
-    </row>
-    <row r="20" spans="1:23" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="7"/>
+      <c r="O20" s="7"/>
+      <c r="P20" s="7"/>
+      <c r="Q20" s="7"/>
+      <c r="R20" s="7"/>
+      <c r="S20" s="7"/>
+      <c r="T20" s="7"/>
+      <c r="U20" s="7"/>
+      <c r="V20" s="7"/>
+      <c r="W20" s="7"/>
+    </row>
+    <row r="21" spans="1:23" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
         <v>63</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C21" t="s">
         <v>45</v>
       </c>
-      <c r="D20" s="18" t="s">
+      <c r="D21" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="H20" s="18"/>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="K20" s="18"/>
-      <c r="L20" s="18"/>
-    </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="D21" s="18"/>
       <c r="E21" s="18"/>
       <c r="F21" s="18"/>
+      <c r="G21" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="H21" s="18"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="K21" s="18"/>
+      <c r="L21" s="18"/>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D22" s="18"/>
@@ -1144,26 +1161,31 @@
       <c r="F22" s="18"/>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B23" s="16" t="s">
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B24" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="C23" s="16" t="s">
+      <c r="C24" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="D23" s="17" t="s">
+      <c r="D24" s="17" t="s">
         <v>47</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="D23:F23"/>
     <mergeCell ref="D1:W1"/>
     <mergeCell ref="G4:H4"/>
-    <mergeCell ref="D20:F20"/>
     <mergeCell ref="D21:F21"/>
+    <mergeCell ref="D22:F22"/>
     <mergeCell ref="I8:J8"/>
-    <mergeCell ref="G20:I20"/>
-    <mergeCell ref="J20:L20"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="J21:L21"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Split BLE data into 2 services
Core Data and Extra Data services created with different update rates (100ms and 500ms respectively)
Updated UUID in "Dashboard BLE Services.xlsx"

Characteristic data names in descriptor disabled
</commit_message>
<xml_diff>
--- a/arduino/Bluetooth/Dashboard BLE Services.xlsx
+++ b/arduino/Bluetooth/Dashboard BLE Services.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sutdapac-my.sharepoint.com/personal/nigel_gomes_mymail_sutd_edu_sg/Documents/Documents/GitHub/evam-dashboard/arduino/Bluetooth/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{615FDA87-1878-4193-8D05-02AAAAB35188}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5666CF65-FDB3-4253-86D4-0686F553FB2B}"/>
+  <xr:revisionPtr revIDLastSave="45" documentId="13_ncr:1_{615FDA87-1878-4193-8D05-02AAAAB35188}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A44EF19D-AC1B-4852-A744-2510987F042A}"/>
   <bookViews>
-    <workbookView xWindow="26940" yWindow="4320" windowWidth="22875" windowHeight="16470" xr2:uid="{07500EA1-3706-482B-9C71-1920CA5A2111}"/>
+    <workbookView xWindow="15525" yWindow="4320" windowWidth="22875" windowHeight="16470" xr2:uid="{07500EA1-3706-482B-9C71-1920CA5A2111}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="76">
   <si>
     <t>Service</t>
   </si>
@@ -162,12 +162,6 @@
     <t>pressure (kPa) = raw data * 4</t>
   </si>
   <si>
-    <t>CAN Bus Node Status</t>
-  </si>
-  <si>
-    <t>TBC</t>
-  </si>
-  <si>
     <t>Lighting</t>
   </si>
   <si>
@@ -225,9 +219,6 @@
     <t>Interior: Hex Colour Value (eg #101010, but without the hashtag)</t>
   </si>
   <si>
-    <t>Lights</t>
-  </si>
-  <si>
     <t>4fafc201-1fb5-459e-8fcc-c5c9c331914b</t>
   </si>
   <si>
@@ -246,7 +237,31 @@
     <t>UUID</t>
   </si>
   <si>
-    <t>Node Status</t>
+    <t>1cbef3f2-12d5-4490-8a80-7f7970b51b54</t>
+  </si>
+  <si>
+    <t>ecu</t>
+  </si>
+  <si>
+    <t>bms</t>
+  </si>
+  <si>
+    <t>tps</t>
+  </si>
+  <si>
+    <t>sas</t>
+  </si>
+  <si>
+    <t>flw</t>
+  </si>
+  <si>
+    <t>frw</t>
+  </si>
+  <si>
+    <t>rrw</t>
+  </si>
+  <si>
+    <t>CANBus Node Status</t>
   </si>
 </sst>
 </file>
@@ -285,20 +300,19 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0" tint="-0.499984740745262"/>
+      <color theme="0" tint="-0.34998626667073579"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="0" tint="-0.499984740745262"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="0" tint="-0.34998626667073579"/>
       <name val="Calibri"/>
@@ -377,7 +391,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
@@ -405,13 +419,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -423,6 +430,16 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -739,125 +756,126 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8933487E-7BF6-40CC-8C7B-EEF7163D084A}">
-  <dimension ref="A1:X24"/>
+  <dimension ref="A1:X23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.85546875" customWidth="1"/>
     <col min="2" max="2" width="42" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" customWidth="1"/>
-    <col min="4" max="4" width="30.42578125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="26.5703125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="23" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="35.42578125" style="4" customWidth="1"/>
-    <col min="10" max="10" width="22.140625" style="4" customWidth="1"/>
-    <col min="11" max="11" width="31.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="23" width="16.28515625" style="4" customWidth="1"/>
-    <col min="24" max="24" width="48.5703125" customWidth="1"/>
+    <col min="3" max="3" width="29.42578125" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" customWidth="1"/>
+    <col min="5" max="5" width="30.42578125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="26.5703125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="23" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="29.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="35.42578125" style="4" customWidth="1"/>
+    <col min="11" max="11" width="22.140625" style="4" customWidth="1"/>
+    <col min="12" max="12" width="31.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="24" width="16.28515625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="1" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="C1" s="3"/>
+      <c r="E1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="19"/>
-      <c r="S1" s="19"/>
-      <c r="T1" s="19"/>
-      <c r="U1" s="19"/>
-      <c r="V1" s="19"/>
-      <c r="W1" s="19"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
+      <c r="V1" s="16"/>
+      <c r="W1" s="16"/>
+      <c r="X1" s="16"/>
     </row>
     <row r="2" spans="1:24" s="2" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="K2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="L2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="M2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="N2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="O2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="P2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="P2" s="5" t="s">
+      <c r="Q2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="Q2" s="5" t="s">
+      <c r="R2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="R2" s="5" t="s">
+      <c r="S2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="S2" s="5" t="s">
+      <c r="T2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="T2" s="5" t="s">
+      <c r="U2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="U2" s="5" t="s">
+      <c r="V2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="V2" s="5" t="s">
+      <c r="W2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="W2" s="5" t="s">
+      <c r="X2" s="5" t="s">
         <v>23</v>
-      </c>
-      <c r="X2" s="2" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:24" s="8" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -865,7 +883,7 @@
         <v>24</v>
       </c>
       <c r="B3" s="12"/>
-      <c r="D3" s="9"/>
+      <c r="C3" s="12"/>
       <c r="E3" s="9"/>
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
@@ -885,27 +903,28 @@
       <c r="U3" s="9"/>
       <c r="V3" s="9"/>
       <c r="W3" s="9"/>
+      <c r="X3" s="9"/>
     </row>
     <row r="4" spans="1:24" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10"/>
       <c r="B4" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="10"/>
+      <c r="D4" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="E4" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="F4" s="11"/>
-      <c r="G4" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="H4" s="20"/>
-      <c r="I4" s="11"/>
+      <c r="F4" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="G4" s="11"/>
+      <c r="H4" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="I4" s="17"/>
       <c r="J4" s="11"/>
       <c r="K4" s="11"/>
       <c r="L4" s="11"/>
@@ -920,12 +939,15 @@
       <c r="U4" s="11"/>
       <c r="V4" s="11"/>
       <c r="W4" s="11"/>
+      <c r="X4" s="11"/>
     </row>
     <row r="7" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="7"/>
+      <c r="C7" s="19" t="s">
+        <v>61</v>
+      </c>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
@@ -945,247 +967,314 @@
       <c r="U7" s="7"/>
       <c r="V7" s="7"/>
       <c r="W7" s="7"/>
-      <c r="X7" s="1" t="s">
-        <v>64</v>
-      </c>
+      <c r="X7" s="7"/>
     </row>
     <row r="8" spans="1:24" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>29</v>
       </c>
       <c r="C8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="E8" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G8" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="H8" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="I8" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="J8" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="K8" s="18"/>
+      <c r="L8" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="G8" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="I8" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="J8" s="21"/>
-      <c r="K8" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="X8" s="6" t="s">
+    </row>
+    <row r="9" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+      <c r="B9" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="H9" s="14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="F10" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="G10" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="H10" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="I10" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="J10" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="K10" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="L10" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="M10" s="22"/>
+      <c r="N10" s="22"/>
+      <c r="O10" s="22"/>
+      <c r="P10" s="22"/>
+      <c r="Q10" s="22"/>
+      <c r="R10" s="22"/>
+      <c r="S10" s="22"/>
+      <c r="T10" s="22"/>
+      <c r="U10" s="22"/>
+      <c r="V10" s="22"/>
+      <c r="W10" s="22"/>
+      <c r="X10" s="22"/>
+    </row>
+    <row r="12" spans="1:24" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="23" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="9" spans="1:24" ht="30" x14ac:dyDescent="0.25">
-      <c r="B9" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="E9" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="F9" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="G9" s="17" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="B10" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-    </row>
-    <row r="12" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7"/>
-      <c r="N12" s="7"/>
-      <c r="O12" s="7"/>
-      <c r="P12" s="7"/>
-      <c r="Q12" s="7"/>
-      <c r="R12" s="7"/>
-      <c r="S12" s="7"/>
-      <c r="T12" s="7"/>
-      <c r="U12" s="7"/>
-      <c r="V12" s="7"/>
-      <c r="W12" s="7"/>
-    </row>
-    <row r="13" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="24"/>
+      <c r="L12" s="24"/>
+      <c r="M12" s="24"/>
+      <c r="N12" s="24"/>
+      <c r="O12" s="24"/>
+      <c r="P12" s="24"/>
+      <c r="Q12" s="24"/>
+      <c r="R12" s="24"/>
+      <c r="S12" s="24"/>
+      <c r="T12" s="24"/>
+      <c r="U12" s="24"/>
+      <c r="V12" s="24"/>
+      <c r="W12" s="24"/>
+      <c r="X12" s="24"/>
+    </row>
+    <row r="13" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B13" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="D13" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="E13" s="14"/>
+      <c r="E13" s="14" t="s">
+        <v>49</v>
+      </c>
       <c r="F13" s="14"/>
       <c r="G13" s="14"/>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="14"/>
+      <c r="N13" s="14"/>
+      <c r="O13" s="14"/>
+      <c r="P13" s="14"/>
+      <c r="Q13" s="14"/>
+      <c r="R13" s="14"/>
+      <c r="S13" s="14"/>
+      <c r="T13" s="14"/>
+      <c r="U13" s="14"/>
+      <c r="V13" s="14"/>
+      <c r="W13" s="14"/>
+      <c r="X13" s="14"/>
+    </row>
+    <row r="14" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B14" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="D14" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="E14" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="E14" s="14" t="s">
+      <c r="F14" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="F14" s="14" t="s">
+      <c r="G14" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="G14" s="14" t="s">
+      <c r="H14" s="14" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="14"/>
+      <c r="N14" s="14"/>
+      <c r="O14" s="14"/>
+      <c r="P14" s="14"/>
+      <c r="Q14" s="14"/>
+      <c r="R14" s="14"/>
+      <c r="S14" s="14"/>
+      <c r="T14" s="14"/>
+      <c r="U14" s="14"/>
+      <c r="V14" s="14"/>
+      <c r="W14" s="14"/>
+      <c r="X14" s="14"/>
+    </row>
+    <row r="15" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B15" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="D15" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="14" t="s">
+      <c r="E15" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="14"/>
       <c r="F15" s="14"/>
       <c r="G15" s="14"/>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="B16" s="13" t="s">
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
+      <c r="N15" s="14"/>
+      <c r="O15" s="14"/>
+      <c r="P15" s="14"/>
+      <c r="Q15" s="14"/>
+      <c r="R15" s="14"/>
+      <c r="S15" s="14"/>
+      <c r="T15" s="14"/>
+      <c r="U15" s="14"/>
+      <c r="V15" s="14"/>
+      <c r="W15" s="14"/>
+      <c r="X15" s="14"/>
+    </row>
+    <row r="19" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="D16" s="15" t="s">
+      <c r="C19" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="7"/>
+      <c r="O19" s="7"/>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="7"/>
+      <c r="R19" s="7"/>
+      <c r="S19" s="7"/>
+      <c r="T19" s="7"/>
+      <c r="U19" s="7"/>
+      <c r="V19" s="7"/>
+      <c r="W19" s="7"/>
+      <c r="X19" s="7"/>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" t="s">
+        <v>64</v>
+      </c>
+      <c r="D20" t="s">
         <v>43</v>
       </c>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-    </row>
-    <row r="20" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
+      <c r="E20" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="I20" s="15"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="L20" s="15"/>
+      <c r="M20" s="15"/>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B23" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="B20" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="7"/>
-      <c r="L20" s="7"/>
-      <c r="M20" s="7"/>
-      <c r="N20" s="7"/>
-      <c r="O20" s="7"/>
-      <c r="P20" s="7"/>
-      <c r="Q20" s="7"/>
-      <c r="R20" s="7"/>
-      <c r="S20" s="7"/>
-      <c r="T20" s="7"/>
-      <c r="U20" s="7"/>
-      <c r="V20" s="7"/>
-      <c r="W20" s="7"/>
-    </row>
-    <row r="21" spans="1:23" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>63</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="D23" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="E23" s="14" t="s">
         <v>45</v>
-      </c>
-      <c r="D21" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="H21" s="18"/>
-      <c r="I21" s="18"/>
-      <c r="J21" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="K21" s="18"/>
-      <c r="L21" s="18"/>
-    </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-    </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-    </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B24" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="C24" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="D24" s="17" t="s">
-        <v>47</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="D1:W1"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="J21:L21"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="E1:X1"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="K20:M20"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Arduino changed battery output range
new format for battery data
</commit_message>
<xml_diff>
--- a/arduino/Bluetooth/Dashboard BLE Services.xlsx
+++ b/arduino/Bluetooth/Dashboard BLE Services.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sutdapac-my.sharepoint.com/personal/nigel_gomes_mymail_sutd_edu_sg/Documents/Documents/GitHub/evam-dashboard/arduino/Bluetooth/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="45" documentId="13_ncr:1_{615FDA87-1878-4193-8D05-02AAAAB35188}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A44EF19D-AC1B-4852-A744-2510987F042A}"/>
+  <xr:revisionPtr revIDLastSave="48" documentId="13_ncr:1_{615FDA87-1878-4193-8D05-02AAAAB35188}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0B0DB897-6927-4E68-9609-B43290B75E22}"/>
   <bookViews>
-    <workbookView xWindow="15525" yWindow="4320" windowWidth="22875" windowHeight="16470" xr2:uid="{07500EA1-3706-482B-9C71-1920CA5A2111}"/>
+    <workbookView xWindow="36154" yWindow="13663" windowWidth="15275" windowHeight="22363" xr2:uid="{07500EA1-3706-482B-9C71-1920CA5A2111}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -207,9 +207,6 @@
     <t>2 bytes can be combined for data range of 0-65535</t>
   </si>
   <si>
-    <t>Batt Current (A) = (MSB * 255 + LSB)/100 (range: 0-65535)</t>
-  </si>
-  <si>
     <t>Front: Hex Colour Value (eg #101010, but without the hashtag)</t>
   </si>
   <si>
@@ -262,6 +259,9 @@
   </si>
   <si>
     <t>CANBus Node Status</t>
+  </si>
+  <si>
+    <t>Batt Current (A) = (MSB * 256 + LSB)/10 - 320 (range: 0-65535)</t>
   </si>
 </sst>
 </file>
@@ -419,6 +419,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -430,16 +440,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -758,61 +758,61 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8933487E-7BF6-40CC-8C7B-EEF7163D084A}">
   <dimension ref="A1:X23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" customWidth="1"/>
+    <col min="1" max="1" width="8.84375" customWidth="1"/>
     <col min="2" max="2" width="42" customWidth="1"/>
-    <col min="3" max="3" width="29.42578125" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" customWidth="1"/>
-    <col min="5" max="5" width="30.42578125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="26.5703125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="29.3828125" customWidth="1"/>
+    <col min="4" max="4" width="20.53515625" customWidth="1"/>
+    <col min="5" max="5" width="30.3828125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="26.53515625" style="4" customWidth="1"/>
     <col min="7" max="7" width="23" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="31.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="29.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="35.42578125" style="4" customWidth="1"/>
-    <col min="11" max="11" width="22.140625" style="4" customWidth="1"/>
-    <col min="12" max="12" width="31.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="24" width="16.28515625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="31.15234375" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="29.53515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="35.3828125" style="4" customWidth="1"/>
+    <col min="11" max="11" width="22.15234375" style="4" customWidth="1"/>
+    <col min="12" max="12" width="31.3828125" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="24" width="16.3046875" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="1" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" s="1" customFormat="1" ht="16.75" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="3"/>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16"/>
-      <c r="P1" s="16"/>
-      <c r="Q1" s="16"/>
-      <c r="R1" s="16"/>
-      <c r="S1" s="16"/>
-      <c r="T1" s="16"/>
-      <c r="U1" s="16"/>
-      <c r="V1" s="16"/>
-      <c r="W1" s="16"/>
-      <c r="X1" s="16"/>
-    </row>
-    <row r="2" spans="1:24" s="2" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
+      <c r="T1" s="22"/>
+      <c r="U1" s="22"/>
+      <c r="V1" s="22"/>
+      <c r="W1" s="22"/>
+      <c r="X1" s="22"/>
+    </row>
+    <row r="2" spans="1:24" s="2" customFormat="1" ht="17.149999999999999" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>3</v>
@@ -878,7 +878,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:24" s="8" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" s="8" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A3" s="12" t="s">
         <v>24</v>
       </c>
@@ -905,7 +905,7 @@
       <c r="W3" s="9"/>
       <c r="X3" s="9"/>
     </row>
-    <row r="4" spans="1:24" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" ht="44.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="10"/>
       <c r="B4" s="10" t="s">
         <v>25</v>
@@ -921,10 +921,10 @@
         <v>46</v>
       </c>
       <c r="G4" s="11"/>
-      <c r="H4" s="17" t="s">
+      <c r="H4" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="I4" s="17"/>
+      <c r="I4" s="23"/>
       <c r="J4" s="11"/>
       <c r="K4" s="11"/>
       <c r="L4" s="11"/>
@@ -941,12 +941,12 @@
       <c r="W4" s="11"/>
       <c r="X4" s="11"/>
     </row>
-    <row r="7" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A7" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="19" t="s">
-        <v>61</v>
+      <c r="C7" s="15" t="s">
+        <v>60</v>
       </c>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
@@ -969,12 +969,12 @@
       <c r="W7" s="7"/>
       <c r="X7" s="7"/>
     </row>
-    <row r="8" spans="1:24" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" ht="14.7" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B8" t="s">
         <v>29</v>
       </c>
       <c r="C8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D8" t="s">
         <v>30</v>
@@ -994,15 +994,15 @@
       <c r="I8" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="J8" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="K8" s="18"/>
+      <c r="J8" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="K8" s="24"/>
       <c r="L8" s="4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" ht="29.15" x14ac:dyDescent="0.4">
       <c r="B9" s="13" t="s">
         <v>31</v>
       </c>
@@ -1022,79 +1022,79 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:24" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="C10" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="D10" s="20" t="s">
+    <row r="10" spans="1:24" s="16" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="B10" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="22" t="s">
+      <c r="E10" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="F10" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="F10" s="22" t="s">
+      <c r="G10" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="G10" s="22" t="s">
+      <c r="H10" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="H10" s="22" t="s">
+      <c r="I10" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="I10" s="22" t="s">
+      <c r="J10" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="J10" s="22" t="s">
+      <c r="K10" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="L10" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="K10" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="L10" s="22" t="s">
-        <v>74</v>
-      </c>
-      <c r="M10" s="22"/>
-      <c r="N10" s="22"/>
-      <c r="O10" s="22"/>
-      <c r="P10" s="22"/>
-      <c r="Q10" s="22"/>
-      <c r="R10" s="22"/>
-      <c r="S10" s="22"/>
-      <c r="T10" s="22"/>
-      <c r="U10" s="22"/>
-      <c r="V10" s="22"/>
-      <c r="W10" s="22"/>
-      <c r="X10" s="22"/>
-    </row>
-    <row r="12" spans="1:24" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="24"/>
-      <c r="I12" s="24"/>
-      <c r="J12" s="24"/>
-      <c r="K12" s="24"/>
-      <c r="L12" s="24"/>
-      <c r="M12" s="24"/>
-      <c r="N12" s="24"/>
-      <c r="O12" s="24"/>
-      <c r="P12" s="24"/>
-      <c r="Q12" s="24"/>
-      <c r="R12" s="24"/>
-      <c r="S12" s="24"/>
-      <c r="T12" s="24"/>
-      <c r="U12" s="24"/>
-      <c r="V12" s="24"/>
-      <c r="W12" s="24"/>
-      <c r="X12" s="24"/>
-    </row>
-    <row r="13" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M10" s="18"/>
+      <c r="N10" s="18"/>
+      <c r="O10" s="18"/>
+      <c r="P10" s="18"/>
+      <c r="Q10" s="18"/>
+      <c r="R10" s="18"/>
+      <c r="S10" s="18"/>
+      <c r="T10" s="18"/>
+      <c r="U10" s="18"/>
+      <c r="V10" s="18"/>
+      <c r="W10" s="18"/>
+      <c r="X10" s="18"/>
+    </row>
+    <row r="12" spans="1:24" s="19" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="20"/>
+      <c r="L12" s="20"/>
+      <c r="M12" s="20"/>
+      <c r="N12" s="20"/>
+      <c r="O12" s="20"/>
+      <c r="P12" s="20"/>
+      <c r="Q12" s="20"/>
+      <c r="R12" s="20"/>
+      <c r="S12" s="20"/>
+      <c r="T12" s="20"/>
+      <c r="U12" s="20"/>
+      <c r="V12" s="20"/>
+      <c r="W12" s="20"/>
+      <c r="X12" s="20"/>
+    </row>
+    <row r="13" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B13" s="13" t="s">
         <v>34</v>
       </c>
@@ -1124,7 +1124,7 @@
       <c r="W13" s="14"/>
       <c r="X13" s="14"/>
     </row>
-    <row r="14" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B14" s="13" t="s">
         <v>35</v>
       </c>
@@ -1160,7 +1160,7 @@
       <c r="W14" s="14"/>
       <c r="X14" s="14"/>
     </row>
-    <row r="15" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B15" s="13" t="s">
         <v>40</v>
       </c>
@@ -1190,12 +1190,12 @@
       <c r="W15" s="14"/>
       <c r="X15" s="14"/>
     </row>
-    <row r="19" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A19" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C19" s="19" t="s">
-        <v>67</v>
+      <c r="C19" s="15" t="s">
+        <v>66</v>
       </c>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
@@ -1218,43 +1218,43 @@
       <c r="W19" s="7"/>
       <c r="X19" s="7"/>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.4">
       <c r="B20" t="s">
         <v>42</v>
       </c>
       <c r="C20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D20" t="s">
         <v>43</v>
       </c>
-      <c r="E20" s="15" t="s">
+      <c r="E20" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="F20" s="21"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="F20" s="15"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="15" t="s">
+      <c r="I20" s="21"/>
+      <c r="J20" s="21"/>
+      <c r="K20" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="I20" s="15"/>
-      <c r="J20" s="15"/>
-      <c r="K20" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="L20" s="15"/>
-      <c r="M20" s="15"/>
-    </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15"/>
-    </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-    </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="L20" s="21"/>
+      <c r="M20" s="21"/>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.4">
+      <c r="E21" s="21"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="21"/>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.4">
+      <c r="E22" s="21"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="21"/>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.4">
       <c r="B23" s="13" t="s">
         <v>44</v>
       </c>

</xml_diff>

<commit_message>
Update UUIDs for new lighting characteristics
</commit_message>
<xml_diff>
--- a/arduino/Bluetooth/Dashboard BLE Services.xlsx
+++ b/arduino/Bluetooth/Dashboard BLE Services.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sutdapac-my.sharepoint.com/personal/nigel_gomes_mymail_sutd_edu_sg/Documents/Documents/GitHub/evam-dashboard/arduino/Bluetooth/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="48" documentId="13_ncr:1_{615FDA87-1878-4193-8D05-02AAAAB35188}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0B0DB897-6927-4E68-9609-B43290B75E22}"/>
+  <xr:revisionPtr revIDLastSave="69" documentId="13_ncr:1_{615FDA87-1878-4193-8D05-02AAAAB35188}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BA19D213-F1BD-4756-95B7-DB60706A2B79}"/>
   <bookViews>
-    <workbookView xWindow="36154" yWindow="13663" windowWidth="15275" windowHeight="22363" xr2:uid="{07500EA1-3706-482B-9C71-1920CA5A2111}"/>
+    <workbookView xWindow="36206" yWindow="6206" windowWidth="15274" windowHeight="22363" xr2:uid="{07500EA1-3706-482B-9C71-1920CA5A2111}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="81">
   <si>
     <t>Service</t>
   </si>
@@ -207,15 +207,6 @@
     <t>2 bytes can be combined for data range of 0-65535</t>
   </si>
   <si>
-    <t>Front: Hex Colour Value (eg #101010, but without the hashtag)</t>
-  </si>
-  <si>
-    <t>Rear: Hex Colour Value (eg #101010, but without the hashtag)</t>
-  </si>
-  <si>
-    <t>Interior: Hex Colour Value (eg #101010, but without the hashtag)</t>
-  </si>
-  <si>
     <t>4fafc201-1fb5-459e-8fcc-c5c9c331914b</t>
   </si>
   <si>
@@ -262,6 +253,30 @@
   </si>
   <si>
     <t>Batt Current (A) = (MSB * 256 + LSB)/10 - 320 (range: 0-65535)</t>
+  </si>
+  <si>
+    <t>Front Lighting</t>
+  </si>
+  <si>
+    <t>Rear Lighting</t>
+  </si>
+  <si>
+    <t>Interior Lighting</t>
+  </si>
+  <si>
+    <t>db598591-bffe-46dd-9967-fbf869e88b3f</t>
+  </si>
+  <si>
+    <t>8ecaaefa-f62f-4376-a4c8-32c74f62d950</t>
+  </si>
+  <si>
+    <t>Red Channel</t>
+  </si>
+  <si>
+    <t>Green Channel</t>
+  </si>
+  <si>
+    <t>Blue Channel</t>
   </si>
 </sst>
 </file>
@@ -391,7 +406,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
@@ -428,9 +443,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -758,8 +770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8933487E-7BF6-40CC-8C7B-EEF7163D084A}">
   <dimension ref="A1:X23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -784,35 +796,35 @@
         <v>0</v>
       </c>
       <c r="C1" s="3"/>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
-      <c r="N1" s="22"/>
-      <c r="O1" s="22"/>
-      <c r="P1" s="22"/>
-      <c r="Q1" s="22"/>
-      <c r="R1" s="22"/>
-      <c r="S1" s="22"/>
-      <c r="T1" s="22"/>
-      <c r="U1" s="22"/>
-      <c r="V1" s="22"/>
-      <c r="W1" s="22"/>
-      <c r="X1" s="22"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
+      <c r="P1" s="21"/>
+      <c r="Q1" s="21"/>
+      <c r="R1" s="21"/>
+      <c r="S1" s="21"/>
+      <c r="T1" s="21"/>
+      <c r="U1" s="21"/>
+      <c r="V1" s="21"/>
+      <c r="W1" s="21"/>
+      <c r="X1" s="21"/>
     </row>
     <row r="2" spans="1:24" s="2" customFormat="1" ht="17.149999999999999" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>3</v>
@@ -921,10 +933,10 @@
         <v>46</v>
       </c>
       <c r="G4" s="11"/>
-      <c r="H4" s="23" t="s">
+      <c r="H4" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="I4" s="23"/>
+      <c r="I4" s="22"/>
       <c r="J4" s="11"/>
       <c r="K4" s="11"/>
       <c r="L4" s="11"/>
@@ -946,7 +958,7 @@
         <v>28</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
@@ -974,7 +986,7 @@
         <v>29</v>
       </c>
       <c r="C8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D8" t="s">
         <v>30</v>
@@ -994,10 +1006,10 @@
       <c r="I8" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="J8" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="K8" s="24"/>
+      <c r="J8" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="K8" s="23"/>
       <c r="L8" s="4" t="s">
         <v>54</v>
       </c>
@@ -1024,37 +1036,37 @@
     </row>
     <row r="10" spans="1:24" s="16" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B10" s="16" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D10" s="16" t="s">
         <v>30</v>
       </c>
       <c r="E10" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="F10" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="G10" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="H10" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="F10" s="18" t="s">
+      <c r="I10" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="G10" s="18" t="s">
+      <c r="J10" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="H10" s="18" t="s">
+      <c r="K10" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="L10" s="18" t="s">
         <v>70</v>
-      </c>
-      <c r="I10" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="J10" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="K10" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="L10" s="18" t="s">
-        <v>73</v>
       </c>
       <c r="M10" s="18"/>
       <c r="N10" s="18"/>
@@ -1071,7 +1083,7 @@
     </row>
     <row r="12" spans="1:24" s="19" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A12" s="19" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E12" s="20"/>
       <c r="F12" s="20"/>
@@ -1195,7 +1207,7 @@
         <v>42</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
@@ -1218,41 +1230,65 @@
       <c r="W19" s="7"/>
       <c r="X19" s="7"/>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:24" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B20" t="s">
-        <v>42</v>
+        <v>73</v>
       </c>
       <c r="C20" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D20" t="s">
         <v>43</v>
       </c>
-      <c r="E20" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="F20" s="21"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="I20" s="21"/>
-      <c r="J20" s="21"/>
-      <c r="K20" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="L20" s="21"/>
-      <c r="M20" s="21"/>
+      <c r="E20" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.4">
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="21"/>
+      <c r="B21" t="s">
+        <v>74</v>
+      </c>
+      <c r="C21" t="s">
+        <v>76</v>
+      </c>
+      <c r="D21" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.4">
-      <c r="E22" s="21"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="21"/>
+      <c r="B22" t="s">
+        <v>75</v>
+      </c>
+      <c r="C22" t="s">
+        <v>77</v>
+      </c>
+      <c r="D22" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.4">
       <c r="B23" s="13" t="s">
@@ -1266,15 +1302,10 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="E22:G22"/>
+  <mergeCells count="3">
     <mergeCell ref="E1:X1"/>
     <mergeCell ref="H4:I4"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="E21:G21"/>
     <mergeCell ref="J8:K8"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="K20:M20"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update Nodes in Excel
</commit_message>
<xml_diff>
--- a/arduino/Bluetooth/Dashboard BLE Services.xlsx
+++ b/arduino/Bluetooth/Dashboard BLE Services.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sutdapac-my.sharepoint.com/personal/nigel_gomes_mymail_sutd_edu_sg/Documents/Documents/GitHub/evam-dashboard/arduino/Bluetooth/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="69" documentId="13_ncr:1_{615FDA87-1878-4193-8D05-02AAAAB35188}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BA19D213-F1BD-4756-95B7-DB60706A2B79}"/>
+  <xr:revisionPtr revIDLastSave="79" documentId="13_ncr:1_{615FDA87-1878-4193-8D05-02AAAAB35188}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6E733A12-C25A-42B9-8D72-841E84F025E3}"/>
   <bookViews>
-    <workbookView xWindow="36206" yWindow="6206" windowWidth="15274" windowHeight="22363" xr2:uid="{07500EA1-3706-482B-9C71-1920CA5A2111}"/>
+    <workbookView xWindow="-5931" yWindow="2991" windowWidth="15274" windowHeight="22363" xr2:uid="{07500EA1-3706-482B-9C71-1920CA5A2111}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="88">
   <si>
     <t>Service</t>
   </si>
@@ -277,6 +277,27 @@
   </si>
   <si>
     <t>Blue Channel</t>
+  </si>
+  <si>
+    <t>rlw</t>
+  </si>
+  <si>
+    <t>fll</t>
+  </si>
+  <si>
+    <t>frl</t>
+  </si>
+  <si>
+    <t>rrl</t>
+  </si>
+  <si>
+    <t>rll</t>
+  </si>
+  <si>
+    <t>imu</t>
+  </si>
+  <si>
+    <t>int</t>
   </si>
 </sst>
 </file>
@@ -770,8 +791,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8933487E-7BF6-40CC-8C7B-EEF7163D084A}">
   <dimension ref="A1:X23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1056,24 +1077,36 @@
       <c r="H10" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="I10" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="J10" s="18" t="s">
-        <v>69</v>
+      <c r="I10" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="J10" s="16" t="s">
+        <v>87</v>
       </c>
       <c r="K10" s="18" t="s">
         <v>68</v>
       </c>
       <c r="L10" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="M10" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="N10" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="M10" s="18"/>
-      <c r="N10" s="18"/>
-      <c r="O10" s="18"/>
-      <c r="P10" s="18"/>
-      <c r="Q10" s="18"/>
-      <c r="R10" s="18"/>
+      <c r="O10" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="P10" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q10" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="R10" s="16" t="s">
+        <v>84</v>
+      </c>
       <c r="S10" s="18"/>
       <c r="T10" s="18"/>
       <c r="U10" s="18"/>

</xml_diff>

<commit_message>
arduino begin canbus development, split status and core services
</commit_message>
<xml_diff>
--- a/arduino/Bluetooth/Dashboard BLE Services.xlsx
+++ b/arduino/Bluetooth/Dashboard BLE Services.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sutdapac-my.sharepoint.com/personal/nigel_gomes_mymail_sutd_edu_sg/Documents/Documents/GitHub/evam-dashboard/arduino/Bluetooth/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="79" documentId="13_ncr:1_{615FDA87-1878-4193-8D05-02AAAAB35188}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6E733A12-C25A-42B9-8D72-841E84F025E3}"/>
+  <xr:revisionPtr revIDLastSave="83" documentId="13_ncr:1_{615FDA87-1878-4193-8D05-02AAAAB35188}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2BE0001C-FDEB-4956-AAE0-75665F8FE89E}"/>
   <bookViews>
-    <workbookView xWindow="-5931" yWindow="2991" windowWidth="15274" windowHeight="22363" xr2:uid="{07500EA1-3706-482B-9C71-1920CA5A2111}"/>
+    <workbookView xWindow="1637" yWindow="2323" windowWidth="15274" windowHeight="22363" xr2:uid="{07500EA1-3706-482B-9C71-1920CA5A2111}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="89">
   <si>
     <t>Service</t>
   </si>
@@ -298,13 +298,16 @@
   </si>
   <si>
     <t>int</t>
+  </si>
+  <si>
+    <t>4ee1bbf0-5e71-4d58-9ce4-e3e45cb8d8f9</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -343,14 +346,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0" tint="-0.34998626667073579"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -427,7 +422,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
@@ -459,10 +454,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -792,7 +783,7 @@
   <dimension ref="A1:X23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -817,28 +808,28 @@
         <v>0</v>
       </c>
       <c r="C1" s="3"/>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="21"/>
-      <c r="O1" s="21"/>
-      <c r="P1" s="21"/>
-      <c r="Q1" s="21"/>
-      <c r="R1" s="21"/>
-      <c r="S1" s="21"/>
-      <c r="T1" s="21"/>
-      <c r="U1" s="21"/>
-      <c r="V1" s="21"/>
-      <c r="W1" s="21"/>
-      <c r="X1" s="21"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
+      <c r="P1" s="19"/>
+      <c r="Q1" s="19"/>
+      <c r="R1" s="19"/>
+      <c r="S1" s="19"/>
+      <c r="T1" s="19"/>
+      <c r="U1" s="19"/>
+      <c r="V1" s="19"/>
+      <c r="W1" s="19"/>
+      <c r="X1" s="19"/>
     </row>
     <row r="2" spans="1:24" s="2" customFormat="1" ht="17.149999999999999" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B2" s="2" t="s">
@@ -954,10 +945,10 @@
         <v>46</v>
       </c>
       <c r="G4" s="11"/>
-      <c r="H4" s="22" t="s">
+      <c r="H4" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="I4" s="22"/>
+      <c r="I4" s="20"/>
       <c r="J4" s="11"/>
       <c r="K4" s="11"/>
       <c r="L4" s="11"/>
@@ -1027,10 +1018,10 @@
       <c r="I8" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="J8" s="23" t="s">
+      <c r="J8" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="K8" s="23"/>
+      <c r="K8" s="21"/>
       <c r="L8" s="4" t="s">
         <v>54</v>
       </c>
@@ -1055,103 +1046,83 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:24" s="16" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="C10" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="D10" s="16" t="s">
+    <row r="11" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="7"/>
+      <c r="R11" s="7"/>
+      <c r="S11" s="7"/>
+      <c r="T11" s="7"/>
+      <c r="U11" s="7"/>
+      <c r="V11" s="7"/>
+      <c r="W11" s="7"/>
+      <c r="X11" s="7"/>
+    </row>
+    <row r="12" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="B12" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="F10" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="G10" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="H10" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="I10" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="J10" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="K10" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="L10" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="M10" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="N10" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="O10" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="P10" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="Q10" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="R10" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="S10" s="18"/>
-      <c r="T10" s="18"/>
-      <c r="U10" s="18"/>
-      <c r="V10" s="18"/>
-      <c r="W10" s="18"/>
-      <c r="X10" s="18"/>
-    </row>
-    <row r="12" spans="1:24" s="19" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="20"/>
-      <c r="J12" s="20"/>
-      <c r="K12" s="20"/>
-      <c r="L12" s="20"/>
-      <c r="M12" s="20"/>
-      <c r="N12" s="20"/>
-      <c r="O12" s="20"/>
-      <c r="P12" s="20"/>
-      <c r="Q12" s="20"/>
-      <c r="R12" s="20"/>
-      <c r="S12" s="20"/>
-      <c r="T12" s="20"/>
-      <c r="U12" s="20"/>
-      <c r="V12" s="20"/>
-      <c r="W12" s="20"/>
-      <c r="X12" s="20"/>
+      <c r="E12" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="14"/>
+      <c r="N12" s="14"/>
+      <c r="O12" s="14"/>
+      <c r="P12" s="14"/>
+      <c r="Q12" s="14"/>
+      <c r="R12" s="14"/>
+      <c r="S12" s="14"/>
+      <c r="T12" s="14"/>
+      <c r="U12" s="14"/>
+      <c r="V12" s="14"/>
+      <c r="W12" s="14"/>
+      <c r="X12" s="14"/>
     </row>
     <row r="13" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B13" s="13" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D13" s="13" t="s">
         <v>30</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
+        <v>36</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="G13" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="H13" s="14" t="s">
+        <v>39</v>
+      </c>
       <c r="I13" s="14"/>
       <c r="J13" s="14"/>
       <c r="K13" s="14"/>
@@ -1171,23 +1142,17 @@
     </row>
     <row r="14" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B14" s="13" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="D14" s="13" t="s">
         <v>30</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="F14" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="G14" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="H14" s="14" t="s">
-        <v>39</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
       <c r="I14" s="14"/>
       <c r="J14" s="14"/>
       <c r="K14" s="14"/>
@@ -1205,35 +1170,64 @@
       <c r="W14" s="14"/>
       <c r="X14" s="14"/>
     </row>
-    <row r="15" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="D15" s="13" t="s">
+    <row r="15" spans="1:24" s="16" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="B15" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="E15" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="14"/>
-      <c r="N15" s="14"/>
-      <c r="O15" s="14"/>
-      <c r="P15" s="14"/>
-      <c r="Q15" s="14"/>
-      <c r="R15" s="14"/>
-      <c r="S15" s="14"/>
-      <c r="T15" s="14"/>
-      <c r="U15" s="14"/>
-      <c r="V15" s="14"/>
-      <c r="W15" s="14"/>
-      <c r="X15" s="14"/>
+      <c r="E15" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="G15" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="H15" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="I15" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="J15" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="K15" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="L15" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="M15" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="N15" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="O15" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="P15" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q15" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="R15" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="S15" s="18"/>
+      <c r="T15" s="18"/>
+      <c r="U15" s="18"/>
+      <c r="V15" s="18"/>
+      <c r="W15" s="18"/>
+      <c r="X15" s="18"/>
     </row>
     <row r="19" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A19" s="6" t="s">

</xml_diff>

<commit_message>
Refactor indicators to not use reanimated shared values
- hopefully saves some ui thread performance
</commit_message>
<xml_diff>
--- a/arduino/Bluetooth/Dashboard BLE Services.xlsx
+++ b/arduino/Bluetooth/Dashboard BLE Services.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\evam-dashboard\arduino\Bluetooth\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFFE9756-F036-4B52-BEDA-EF791ABCCD0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{798F3C61-B497-4879-937A-013DB8FEADDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{07500EA1-3706-482B-9C71-1920CA5A2111}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="92">
   <si>
     <t>Service</t>
   </si>
@@ -307,6 +307,9 @@
   </si>
   <si>
     <t>3a9a4b03-75a4-48fb-a071-af568425664e</t>
+  </si>
+  <si>
+    <t>whl</t>
   </si>
 </sst>
 </file>
@@ -371,7 +374,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -408,21 +411,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
@@ -455,9 +449,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -778,8 +769,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8933487E-7BF6-40CC-8C7B-EEF7163D084A}">
   <dimension ref="A1:X23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1008,19 +999,11 @@
       <c r="G8" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="H8" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="J8" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="K8" s="18"/>
-      <c r="L8" s="4" t="s">
-        <v>54</v>
-      </c>
+      <c r="T8"/>
+      <c r="U8"/>
+      <c r="V8"/>
+      <c r="W8"/>
+      <c r="X8"/>
     </row>
     <row r="9" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" s="13" t="s">
@@ -1188,37 +1171,39 @@
       <c r="H15" t="s">
         <v>67</v>
       </c>
-      <c r="I15" t="s">
+      <c r="I15" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="J15" t="s">
         <v>86</v>
       </c>
-      <c r="J15" t="s">
+      <c r="K15" t="s">
         <v>87</v>
       </c>
-      <c r="K15" t="s">
+      <c r="L15" t="s">
         <v>68</v>
       </c>
-      <c r="L15" t="s">
+      <c r="M15" t="s">
         <v>69</v>
       </c>
-      <c r="M15" t="s">
+      <c r="N15" t="s">
         <v>81</v>
       </c>
-      <c r="N15" t="s">
+      <c r="O15" t="s">
         <v>70</v>
       </c>
-      <c r="O15" t="s">
+      <c r="P15" t="s">
         <v>82</v>
       </c>
-      <c r="P15" t="s">
+      <c r="Q15" t="s">
         <v>83</v>
       </c>
-      <c r="Q15" t="s">
+      <c r="R15" t="s">
         <v>85</v>
       </c>
-      <c r="R15" t="s">
+      <c r="S15" t="s">
         <v>84</v>
       </c>
-      <c r="S15"/>
       <c r="T15"/>
       <c r="U15"/>
       <c r="V15"/>
@@ -1241,10 +1226,10 @@
       <c r="F16" t="s">
         <v>55</v>
       </c>
-      <c r="G16" s="19" t="s">
+      <c r="G16" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="H16" s="19"/>
+      <c r="H16" s="18"/>
       <c r="I16" t="s">
         <v>54</v>
       </c>
@@ -1364,10 +1349,9 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="3">
     <mergeCell ref="E1:X1"/>
     <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J8:K8"/>
     <mergeCell ref="G16:H16"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>

<commit_message>
Update Arduino TPS node code
</commit_message>
<xml_diff>
--- a/arduino/Bluetooth/Dashboard BLE Services.xlsx
+++ b/arduino/Bluetooth/Dashboard BLE Services.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\evam-dashboard\arduino\Bluetooth\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sutdapac-my.sharepoint.com/personal/nigel_gomes_mymail_sutd_edu_sg/Documents/Documents/GitHub/evam-dashboard/arduino/Bluetooth/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{798F3C61-B497-4879-937A-013DB8FEADDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{798F3C61-B497-4879-937A-013DB8FEADDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CDD9FA1D-47DD-4FEC-9EE2-96BFDBF580D1}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{07500EA1-3706-482B-9C71-1920CA5A2111}"/>
+    <workbookView xWindow="2880" yWindow="1950" windowWidth="22875" windowHeight="16470" xr2:uid="{07500EA1-3706-482B-9C71-1920CA5A2111}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -769,8 +769,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8933487E-7BF6-40CC-8C7B-EEF7163D084A}">
   <dimension ref="A1:X23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J36" sqref="J36"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -780,8 +780,8 @@
     <col min="3" max="3" width="29.42578125" customWidth="1"/>
     <col min="4" max="4" width="20.5703125" customWidth="1"/>
     <col min="5" max="5" width="30.42578125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="26.5703125" style="4" customWidth="1"/>
-    <col min="7" max="7" width="23" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.5703125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="28.5703125" style="4" customWidth="1"/>
     <col min="8" max="8" width="31.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="29.5703125" style="4" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="35.42578125" style="4" customWidth="1"/>

</xml_diff>

<commit_message>
Update TPS and BMS code for Adruino, update BLE Services.xlsx
</commit_message>
<xml_diff>
--- a/arduino/Bluetooth/Dashboard BLE Services.xlsx
+++ b/arduino/Bluetooth/Dashboard BLE Services.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sutdapac-my.sharepoint.com/personal/nigel_gomes_mymail_sutd_edu_sg/Documents/Documents/GitHub/evam-dashboard/arduino/Bluetooth/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{798F3C61-B497-4879-937A-013DB8FEADDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CDD9FA1D-47DD-4FEC-9EE2-96BFDBF580D1}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="13_ncr:1_{798F3C61-B497-4879-937A-013DB8FEADDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6505EF4E-83D7-45F8-B567-8DE32B0F4C50}"/>
   <bookViews>
-    <workbookView xWindow="2880" yWindow="1950" windowWidth="22875" windowHeight="16470" xr2:uid="{07500EA1-3706-482B-9C71-1920CA5A2111}"/>
+    <workbookView minimized="1" xWindow="15525" yWindow="5130" windowWidth="22875" windowHeight="16470" xr2:uid="{07500EA1-3706-482B-9C71-1920CA5A2111}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="88">
   <si>
     <t>Service</t>
   </si>
@@ -231,24 +231,6 @@
     <t>ecu</t>
   </si>
   <si>
-    <t>bms</t>
-  </si>
-  <si>
-    <t>tps</t>
-  </si>
-  <si>
-    <t>sas</t>
-  </si>
-  <si>
-    <t>flw</t>
-  </si>
-  <si>
-    <t>frw</t>
-  </si>
-  <si>
-    <t>rrw</t>
-  </si>
-  <si>
     <t>CANBus Node Status</t>
   </si>
   <si>
@@ -279,27 +261,6 @@
     <t>Blue Channel</t>
   </si>
   <si>
-    <t>rlw</t>
-  </si>
-  <si>
-    <t>fll</t>
-  </si>
-  <si>
-    <t>frl</t>
-  </si>
-  <si>
-    <t>rrl</t>
-  </si>
-  <si>
-    <t>rll</t>
-  </si>
-  <si>
-    <t>imu</t>
-  </si>
-  <si>
-    <t>int</t>
-  </si>
-  <si>
     <t>4ee1bbf0-5e71-4d58-9ce4-e3e45cb8d8f9</t>
   </si>
   <si>
@@ -309,7 +270,34 @@
     <t>3a9a4b03-75a4-48fb-a071-af568425664e</t>
   </si>
   <si>
-    <t>whl</t>
+    <t>fl (front light)</t>
+  </si>
+  <si>
+    <t>rl (rear light)</t>
+  </si>
+  <si>
+    <t>int (interior light)</t>
+  </si>
+  <si>
+    <t>fw (front wheels)</t>
+  </si>
+  <si>
+    <t>rlw (rear left wheel)</t>
+  </si>
+  <si>
+    <t>rrw (rear right wheel)</t>
+  </si>
+  <si>
+    <t>imu (inertial measurment unit)</t>
+  </si>
+  <si>
+    <t>sas (steering angle sensor)</t>
+  </si>
+  <si>
+    <t>tps (throttle and brake position sensor)</t>
+  </si>
+  <si>
+    <t>bms (battery management system)</t>
   </si>
 </sst>
 </file>
@@ -769,8 +757,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8933487E-7BF6-40CC-8C7B-EEF7163D084A}">
   <dimension ref="A1:X23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1030,7 +1018,7 @@
         <v>61</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
@@ -1151,7 +1139,7 @@
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C15" t="s">
         <v>59</v>
@@ -1163,47 +1151,39 @@
         <v>64</v>
       </c>
       <c r="F15" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="G15" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="H15" t="s">
-        <v>67</v>
-      </c>
-      <c r="I15" s="4" t="s">
-        <v>91</v>
+        <v>85</v>
+      </c>
+      <c r="I15" t="s">
+        <v>84</v>
       </c>
       <c r="J15" t="s">
-        <v>86</v>
-      </c>
-      <c r="K15" t="s">
-        <v>87</v>
+        <v>81</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>82</v>
       </c>
       <c r="L15" t="s">
-        <v>68</v>
+        <v>83</v>
       </c>
       <c r="M15" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="N15" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="O15" t="s">
-        <v>70</v>
-      </c>
-      <c r="P15" t="s">
-        <v>82</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>83</v>
-      </c>
-      <c r="R15" t="s">
-        <v>85</v>
-      </c>
-      <c r="S15" t="s">
-        <v>84</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="P15"/>
+      <c r="Q15"/>
+      <c r="R15"/>
+      <c r="S15"/>
       <c r="T15"/>
       <c r="U15"/>
       <c r="V15"/>
@@ -1212,10 +1192,10 @@
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="C16" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="D16" t="s">
         <v>30</v>
@@ -1227,7 +1207,7 @@
         <v>55</v>
       </c>
       <c r="G16" s="18" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="H16" s="18"/>
       <c r="I16" t="s">
@@ -1279,7 +1259,7 @@
     </row>
     <row r="20" spans="1:24" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C20" t="s">
         <v>60</v>
@@ -1288,53 +1268,53 @@
         <v>43</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C21" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D21" t="s">
         <v>43</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C22" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D22" t="s">
         <v>43</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update description and can_ids
</commit_message>
<xml_diff>
--- a/arduino/Bluetooth/Dashboard BLE Services.xlsx
+++ b/arduino/Bluetooth/Dashboard BLE Services.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sutdapac-my.sharepoint.com/personal/nigel_gomes_mymail_sutd_edu_sg/Documents/Documents/GitHub/evam-dashboard/arduino/Bluetooth/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="13_ncr:1_{798F3C61-B497-4879-937A-013DB8FEADDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6505EF4E-83D7-45F8-B567-8DE32B0F4C50}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="13_ncr:1_{798F3C61-B497-4879-937A-013DB8FEADDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9EF7F938-80A8-4B6B-9147-5BDC84EA5A6B}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="15525" yWindow="5130" windowWidth="22875" windowHeight="16470" xr2:uid="{07500EA1-3706-482B-9C71-1920CA5A2111}"/>
+    <workbookView xWindow="1534" yWindow="-103" windowWidth="25997" windowHeight="15634" xr2:uid="{07500EA1-3706-482B-9C71-1920CA5A2111}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -757,28 +757,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8933487E-7BF6-40CC-8C7B-EEF7163D084A}">
   <dimension ref="A1:X23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16:H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" customWidth="1"/>
+    <col min="1" max="1" width="8.84375" customWidth="1"/>
     <col min="2" max="2" width="42" customWidth="1"/>
-    <col min="3" max="3" width="29.42578125" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" customWidth="1"/>
-    <col min="5" max="5" width="30.42578125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="33.5703125" style="4" customWidth="1"/>
-    <col min="7" max="7" width="28.5703125" style="4" customWidth="1"/>
-    <col min="8" max="8" width="31.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="29.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="35.42578125" style="4" customWidth="1"/>
-    <col min="11" max="11" width="22.140625" style="4" customWidth="1"/>
-    <col min="12" max="12" width="31.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="24" width="16.28515625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="29.3828125" customWidth="1"/>
+    <col min="4" max="4" width="20.53515625" customWidth="1"/>
+    <col min="5" max="5" width="30.3828125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="33.53515625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="28.53515625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="31.15234375" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="29.53515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="35.3828125" style="4" customWidth="1"/>
+    <col min="11" max="11" width="22.15234375" style="4" customWidth="1"/>
+    <col min="12" max="12" width="31.3828125" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="24" width="16.3046875" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="1" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" s="1" customFormat="1" ht="16.75" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -806,7 +806,7 @@
       <c r="W1" s="16"/>
       <c r="X1" s="16"/>
     </row>
-    <row r="2" spans="1:24" s="2" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:24" s="2" customFormat="1" ht="17.149999999999999" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
@@ -877,7 +877,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:24" s="8" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" s="8" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A3" s="12" t="s">
         <v>24</v>
       </c>
@@ -904,7 +904,7 @@
       <c r="W3" s="9"/>
       <c r="X3" s="9"/>
     </row>
-    <row r="4" spans="1:24" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" ht="44.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="10"/>
       <c r="B4" s="10" t="s">
         <v>25</v>
@@ -940,7 +940,7 @@
       <c r="W4" s="11"/>
       <c r="X4" s="11"/>
     </row>
-    <row r="7" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A7" s="6" t="s">
         <v>28</v>
       </c>
@@ -968,7 +968,7 @@
       <c r="W7" s="7"/>
       <c r="X7" s="7"/>
     </row>
-    <row r="8" spans="1:24" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" ht="14.7" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B8" t="s">
         <v>29</v>
       </c>
@@ -993,7 +993,7 @@
       <c r="W8"/>
       <c r="X8"/>
     </row>
-    <row r="9" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" ht="29.15" x14ac:dyDescent="0.4">
       <c r="B9" s="13" t="s">
         <v>31</v>
       </c>
@@ -1013,7 +1013,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A11" s="6" t="s">
         <v>61</v>
       </c>
@@ -1041,7 +1041,7 @@
       <c r="W11" s="7"/>
       <c r="X11" s="7"/>
     </row>
-    <row r="12" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B12" s="13" t="s">
         <v>34</v>
       </c>
@@ -1071,7 +1071,7 @@
       <c r="W12" s="14"/>
       <c r="X12" s="14"/>
     </row>
-    <row r="13" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B13" s="13" t="s">
         <v>35</v>
       </c>
@@ -1107,7 +1107,7 @@
       <c r="W13" s="14"/>
       <c r="X13" s="14"/>
     </row>
-    <row r="14" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B14" s="13" t="s">
         <v>40</v>
       </c>
@@ -1137,7 +1137,7 @@
       <c r="W14" s="14"/>
       <c r="X14" s="14"/>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.4">
       <c r="B15" t="s">
         <v>65</v>
       </c>
@@ -1190,7 +1190,7 @@
       <c r="W15"/>
       <c r="X15"/>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.4">
       <c r="B16" t="s">
         <v>76</v>
       </c>
@@ -1229,7 +1229,7 @@
       <c r="W16"/>
       <c r="X16"/>
     </row>
-    <row r="19" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A19" s="6" t="s">
         <v>42</v>
       </c>
@@ -1257,7 +1257,7 @@
       <c r="W19" s="7"/>
       <c r="X19" s="7"/>
     </row>
-    <row r="20" spans="1:24" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24" ht="14.7" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B20" t="s">
         <v>67</v>
       </c>
@@ -1277,7 +1277,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.4">
       <c r="B21" t="s">
         <v>68</v>
       </c>
@@ -1297,7 +1297,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.4">
       <c r="B22" t="s">
         <v>69</v>
       </c>
@@ -1317,7 +1317,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.4">
       <c r="B23" s="13" t="s">
         <v>44</v>
       </c>

</xml_diff>

<commit_message>
Add reverse indicator, battery temperature
</commit_message>
<xml_diff>
--- a/arduino/Bluetooth/Dashboard BLE Services.xlsx
+++ b/arduino/Bluetooth/Dashboard BLE Services.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sutdapac-my.sharepoint.com/personal/nigel_gomes_mymail_sutd_edu_sg/Documents/Documents/GitHub/evam-dashboard/arduino/Bluetooth/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nigel\Documents\GitHub\evam-dashboard\arduino\Bluetooth\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="13_ncr:1_{798F3C61-B497-4879-937A-013DB8FEADDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9EF7F938-80A8-4B6B-9147-5BDC84EA5A6B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{478DC211-3E8B-4833-9855-BEFC56F27D4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1534" yWindow="-103" windowWidth="25997" windowHeight="15634" xr2:uid="{07500EA1-3706-482B-9C71-1920CA5A2111}"/>
+    <workbookView xWindow="874" yWindow="-103" windowWidth="26657" windowHeight="15634" xr2:uid="{07500EA1-3706-482B-9C71-1920CA5A2111}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="89">
   <si>
     <t>Service</t>
   </si>
@@ -298,6 +298,9 @@
   </si>
   <si>
     <t>bms (battery management system)</t>
+  </si>
+  <si>
+    <t>Reverse = 0 (drive) or 1 (reverse)</t>
   </si>
 </sst>
 </file>
@@ -432,7 +435,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -758,7 +761,7 @@
   <dimension ref="A1:X23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16:H16"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -987,6 +990,9 @@
       <c r="G8" s="4" t="s">
         <v>52</v>
       </c>
+      <c r="H8" s="4" t="s">
+        <v>88</v>
+      </c>
       <c r="T8"/>
       <c r="U8"/>
       <c r="V8"/>

</xml_diff>

<commit_message>
add steering angle to bluetooth
- include SAS angle in the bluetooth data under Core Data
</commit_message>
<xml_diff>
--- a/arduino/Bluetooth/Dashboard BLE Services.xlsx
+++ b/arduino/Bluetooth/Dashboard BLE Services.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nigel\Documents\GitHub\evam-dashboard\arduino\Bluetooth\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{478DC211-3E8B-4833-9855-BEFC56F27D4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81CB4388-2A74-4C5A-A3C4-0F3FF655158A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="874" yWindow="-103" windowWidth="26657" windowHeight="15634" xr2:uid="{07500EA1-3706-482B-9C71-1920CA5A2111}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="87">
   <si>
     <t>Service</t>
   </si>
@@ -138,9 +138,6 @@
     <t>Errors, if any (As ASCII text) (variable length)</t>
   </si>
   <si>
-    <t>Steering Wheel angle</t>
-  </si>
-  <si>
     <t>Wheel Speeds</t>
   </si>
   <si>
@@ -180,12 +177,6 @@
     <t>Locked = 0 Unlocked = 1</t>
   </si>
   <si>
-    <t>Forward = 0 Reverse = 1</t>
-  </si>
-  <si>
-    <t>Angle (in deg) = raw data-128</t>
-  </si>
-  <si>
     <t>Speed (in km/h) = raw data (0-255)</t>
   </si>
   <si>
@@ -301,6 +292,9 @@
   </si>
   <si>
     <t>Reverse = 0 (drive) or 1 (reverse)</t>
+  </si>
+  <si>
+    <t>Steering Angle. For now: 0 left lock, 128 centre, 255 right lock</t>
   </si>
 </sst>
 </file>
@@ -758,10 +752,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8933487E-7BF6-40CC-8C7B-EEF7163D084A}">
-  <dimension ref="A1:X23"/>
+  <dimension ref="A1:X22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -814,7 +808,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>3</v>
@@ -920,11 +914,11 @@
         <v>27</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G4" s="11"/>
       <c r="H4" s="17" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="I4" s="17"/>
       <c r="J4" s="11"/>
@@ -948,7 +942,7 @@
         <v>28</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
@@ -976,22 +970,25 @@
         <v>29</v>
       </c>
       <c r="C8" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D8" t="s">
         <v>30</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>88</v>
+        <v>85</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>86</v>
       </c>
       <c r="T8"/>
       <c r="U8"/>
@@ -1007,24 +1004,21 @@
         <v>30</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F9" s="14" t="s">
         <v>32</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="H9" s="14" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A11" s="6" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
@@ -1055,11 +1049,17 @@
         <v>30</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
+        <v>35</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="G12" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="H12" s="14" t="s">
+        <v>38</v>
+      </c>
       <c r="I12" s="14"/>
       <c r="J12" s="14"/>
       <c r="K12" s="14"/>
@@ -1079,23 +1079,17 @@
     </row>
     <row r="13" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B13" s="13" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D13" s="13" t="s">
         <v>30</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="F13" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="G13" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="H13" s="14" t="s">
-        <v>39</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
       <c r="I13" s="14"/>
       <c r="J13" s="14"/>
       <c r="K13" s="14"/>
@@ -1113,79 +1107,88 @@
       <c r="W13" s="14"/>
       <c r="X13" s="14"/>
     </row>
-    <row r="14" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="D14" s="13" t="s">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.4">
+      <c r="B14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" t="s">
+        <v>56</v>
+      </c>
+      <c r="D14" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="14"/>
-      <c r="N14" s="14"/>
-      <c r="O14" s="14"/>
-      <c r="P14" s="14"/>
-      <c r="Q14" s="14"/>
-      <c r="R14" s="14"/>
-      <c r="S14" s="14"/>
-      <c r="T14" s="14"/>
-      <c r="U14" s="14"/>
-      <c r="V14" s="14"/>
-      <c r="W14" s="14"/>
-      <c r="X14" s="14"/>
+      <c r="E14" t="s">
+        <v>61</v>
+      </c>
+      <c r="F14" t="s">
+        <v>84</v>
+      </c>
+      <c r="G14" t="s">
+        <v>83</v>
+      </c>
+      <c r="H14" t="s">
+        <v>82</v>
+      </c>
+      <c r="I14" t="s">
+        <v>81</v>
+      </c>
+      <c r="J14" t="s">
+        <v>78</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="L14" t="s">
+        <v>80</v>
+      </c>
+      <c r="M14" t="s">
+        <v>75</v>
+      </c>
+      <c r="N14" t="s">
+        <v>76</v>
+      </c>
+      <c r="O14" t="s">
+        <v>77</v>
+      </c>
+      <c r="P14"/>
+      <c r="Q14"/>
+      <c r="R14"/>
+      <c r="S14"/>
+      <c r="T14"/>
+      <c r="U14"/>
+      <c r="V14"/>
+      <c r="W14"/>
+      <c r="X14"/>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.4">
       <c r="B15" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="C15" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="D15" t="s">
         <v>30</v>
       </c>
       <c r="E15" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="F15" t="s">
-        <v>87</v>
-      </c>
-      <c r="G15" t="s">
-        <v>86</v>
-      </c>
-      <c r="H15" t="s">
-        <v>85</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="G15" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="H15" s="18"/>
       <c r="I15" t="s">
-        <v>84</v>
-      </c>
-      <c r="J15" t="s">
-        <v>81</v>
-      </c>
-      <c r="K15" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="L15" t="s">
-        <v>83</v>
-      </c>
-      <c r="M15" t="s">
-        <v>78</v>
-      </c>
-      <c r="N15" t="s">
-        <v>79</v>
-      </c>
-      <c r="O15" t="s">
-        <v>80</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="J15"/>
+      <c r="K15"/>
+      <c r="L15"/>
+      <c r="M15"/>
+      <c r="N15"/>
+      <c r="O15"/>
       <c r="P15"/>
       <c r="Q15"/>
       <c r="R15"/>
@@ -1196,149 +1199,110 @@
       <c r="W15"/>
       <c r="X15"/>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.4">
-      <c r="B16" t="s">
-        <v>76</v>
-      </c>
-      <c r="C16" t="s">
-        <v>77</v>
-      </c>
-      <c r="D16" t="s">
-        <v>30</v>
-      </c>
-      <c r="E16" t="s">
-        <v>53</v>
-      </c>
-      <c r="F16" t="s">
-        <v>55</v>
-      </c>
-      <c r="G16" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="H16" s="18"/>
-      <c r="I16" t="s">
-        <v>54</v>
-      </c>
-      <c r="J16"/>
-      <c r="K16"/>
-      <c r="L16"/>
-      <c r="M16"/>
-      <c r="N16"/>
-      <c r="O16"/>
-      <c r="P16"/>
-      <c r="Q16"/>
-      <c r="R16"/>
-      <c r="S16"/>
-      <c r="T16"/>
-      <c r="U16"/>
-      <c r="V16"/>
-      <c r="W16"/>
-      <c r="X16"/>
-    </row>
-    <row r="19" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="6" t="s">
+    <row r="18" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="7"/>
+      <c r="N18" s="7"/>
+      <c r="O18" s="7"/>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="7"/>
+      <c r="R18" s="7"/>
+      <c r="S18" s="7"/>
+      <c r="T18" s="7"/>
+      <c r="U18" s="7"/>
+      <c r="V18" s="7"/>
+      <c r="W18" s="7"/>
+      <c r="X18" s="7"/>
+    </row>
+    <row r="19" spans="1:24" ht="14.7" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B19" t="s">
+        <v>64</v>
+      </c>
+      <c r="C19" t="s">
+        <v>57</v>
+      </c>
+      <c r="D19" t="s">
         <v>42</v>
       </c>
-      <c r="C19" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="7"/>
-      <c r="L19" s="7"/>
-      <c r="M19" s="7"/>
-      <c r="N19" s="7"/>
-      <c r="O19" s="7"/>
-      <c r="P19" s="7"/>
-      <c r="Q19" s="7"/>
-      <c r="R19" s="7"/>
-      <c r="S19" s="7"/>
-      <c r="T19" s="7"/>
-      <c r="U19" s="7"/>
-      <c r="V19" s="7"/>
-      <c r="W19" s="7"/>
-      <c r="X19" s="7"/>
-    </row>
-    <row r="20" spans="1:24" ht="14.7" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="E19" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.4">
       <c r="B20" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" t="s">
         <v>67</v>
       </c>
-      <c r="C20" t="s">
-        <v>60</v>
-      </c>
       <c r="D20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.4">
       <c r="B21" t="s">
+        <v>66</v>
+      </c>
+      <c r="C21" t="s">
         <v>68</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
+        <v>42</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="F21" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="D21" t="s">
+      <c r="G21" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.4">
+      <c r="B22" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="E21" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.4">
-      <c r="B22" t="s">
-        <v>69</v>
-      </c>
-      <c r="C22" t="s">
-        <v>71</v>
-      </c>
-      <c r="D22" t="s">
-        <v>43</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.4">
-      <c r="B23" s="13" t="s">
+      <c r="D22" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E22" s="14" t="s">
         <v>44</v>
-      </c>
-      <c r="D23" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="E23" s="14" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="E1:X1"/>
     <mergeCell ref="H4:I4"/>
-    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="G15:H15"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>